<commit_message>
feat: continue developing - add hmi and telemetry components - work in progress
</commit_message>
<xml_diff>
--- a/PINOUT.xlsx
+++ b/PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Projects\WS_Solarium_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B89DB53-055F-4B20-AD88-7138EB3C3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F90898-5DCC-4121-849E-EB7B869A25EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28365" windowHeight="15345" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
+    <workbookView xWindow="25920" yWindow="3405" windowWidth="12480" windowHeight="15345" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
   <si>
     <t>GPIO1</t>
   </si>
@@ -213,9 +216,6 @@
     <t>SPIQ MISO</t>
   </si>
   <si>
-    <t>UART - PMS5003</t>
-  </si>
-  <si>
     <t>ADC2</t>
   </si>
   <si>
@@ -297,18 +297,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>PWM - mosfet - valve 1</t>
-  </si>
-  <si>
-    <t>PWM - mosfet - valve 2</t>
-  </si>
-  <si>
-    <t>PWM - mosfet - valve 3</t>
-  </si>
-  <si>
-    <t>PWM - mosfet - valve 4</t>
-  </si>
-  <si>
     <t>SN74AHCT125</t>
   </si>
   <si>
@@ -318,140 +306,124 @@
     <t>PWM - case cooling fan</t>
   </si>
   <si>
+    <t>ADS1115 ADC 3 CH. 1 - MT</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 3 CH. 3 - FREE</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 3 CH. 2 - PT - pump</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 1 CH. 4 - PR</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 1 CH. 3 - PR</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 1 CH. 2 - PR</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 1 CH. 1 - PR</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin </t>
+  </si>
+  <si>
+    <t>Intended use</t>
+  </si>
+  <si>
+    <t>PULSE - FT OF05ZAT</t>
+  </si>
+  <si>
+    <t>Boot Strapping Pin</t>
+  </si>
+  <si>
+    <t>Warnings:</t>
+  </si>
+  <si>
+    <t>Flash-Connected Pin</t>
+  </si>
+  <si>
+    <t>UART0 Pin</t>
+  </si>
+  <si>
+    <t>BOTH Boot/Flash</t>
+  </si>
+  <si>
+    <t>SN74AHCT125's OE #1</t>
+  </si>
+  <si>
+    <t>SN74AHCT125's OE #2</t>
+  </si>
+  <si>
+    <t>HALL DI - Rainfall Water input</t>
+  </si>
+  <si>
+    <t>HALL DI - Rain Tipbucket</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 4 CH. 1 - HALL</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 4 CH. 2 - HALL</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 4 CH. 3 - HALL</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 4 CH. 4 - HALL</t>
+  </si>
+  <si>
+    <t>SPI DC - OLED</t>
+  </si>
+  <si>
     <t>?</t>
   </si>
   <si>
-    <t>MOSFET</t>
-  </si>
-  <si>
-    <t>CUTOFF</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 1 - MT</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 3 - FREE</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 2 - PT - pump</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 1 CH. 4 - PR</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 1 CH. 3 - PR</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 1 CH. 2 - PR</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 1 CH. 1 - PR</t>
-  </si>
-  <si>
-    <t>PWM - mosfet - PUMP</t>
-  </si>
-  <si>
-    <t>PWM - mosfet - valve 5</t>
-  </si>
-  <si>
-    <t>12 V</t>
-  </si>
-  <si>
-    <t>CUTOFFs</t>
-  </si>
-  <si>
-    <t>3.3 V</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">CUTOFF </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6.2 V</t>
-    </r>
-  </si>
-  <si>
-    <t>6 total</t>
-  </si>
-  <si>
-    <t>1 mosfet</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin </t>
-  </si>
-  <si>
-    <t>Intended use</t>
-  </si>
-  <si>
-    <t>PULSE - FT OF05ZAT</t>
-  </si>
-  <si>
-    <t>INDIVIDUAL mosfet</t>
-  </si>
-  <si>
-    <t>Boot Strapping Pin</t>
-  </si>
-  <si>
-    <t>Warnings:</t>
-  </si>
-  <si>
-    <t>Flash-Connected Pin</t>
-  </si>
-  <si>
-    <t>UART0 Pin</t>
-  </si>
-  <si>
-    <t>BOTH Boot/Flash</t>
-  </si>
-  <si>
-    <t>CUTOFF 12 V single</t>
-  </si>
-  <si>
-    <t>SN74AHCT125's OE #1</t>
-  </si>
-  <si>
-    <t>SN74AHCT125's OE #2</t>
-  </si>
-  <si>
-    <t>SN74AHCT125's OE #3</t>
-  </si>
-  <si>
-    <t>5 V shared cutoff</t>
-  </si>
-  <si>
-    <t>by mosfet</t>
-  </si>
-  <si>
-    <t>3V3_SENSOR_BUS_CUTOFF</t>
-  </si>
-  <si>
-    <t>5V_SENSOR_BUS_CUTOFF</t>
-  </si>
-  <si>
-    <t>SERVO_BUS_CUTOFF</t>
-  </si>
-  <si>
-    <t>HALL DI - Rainfall Water input</t>
-  </si>
-  <si>
-    <t>HALL DI - Rain Tipbucket</t>
-  </si>
-  <si>
-    <t>PWM - servo - shared cutoff</t>
-  </si>
-  <si>
-    <t>12V_BUS_CUTOFF</t>
+    <t>12V_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>6V6_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>5V_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>3V3_SENSOR_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 5</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 4</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 3</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 2</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 1</t>
+  </si>
+  <si>
+    <t>MOSFET - PWM PUMP</t>
+  </si>
+  <si>
+    <t>UART TX - PMS5003</t>
+  </si>
+  <si>
+    <t>UART RX - PMS5003</t>
+  </si>
+  <si>
+    <t>PWM - SERVO - PITCH CTRL</t>
+  </si>
+  <si>
+    <t>PWM - SERVO - YAW CTRL</t>
   </si>
 </sst>
 </file>
@@ -510,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,12 +515,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -615,12 +581,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -649,8 +609,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA66BD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBF94E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5B6EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDFBD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F0F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -808,13 +798,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color theme="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -826,10 +868,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -837,58 +878,59 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,15 +939,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFF3F0F4"/>
+      <color rgb="FFFDFBD3"/>
+      <color rgb="FFD5B6EC"/>
+      <color rgb="FFBF94E0"/>
+      <color rgb="FFDAC0EE"/>
+      <color rgb="FFA66BD3"/>
       <color rgb="FF85FFBC"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FF7CB854"/>
       <color rgb="FF3B9B40"/>
-      <color rgb="FFC9E2B8"/>
-      <color rgb="FF5CF2A0"/>
-      <color rgb="FFEADBF5"/>
-      <color rgb="FFD5B8EA"/>
-      <color rgb="FFB07BD7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1216,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986543E9-FEEA-4416-9297-1960C94E5E52}">
-  <dimension ref="A1:T63"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,6 +1274,7 @@
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" customWidth="1"/>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
     <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -1238,708 +1282,702 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="E2" s="59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="D2" s="52" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>123</v>
+      <c r="D3" s="31" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
-        <v>117</v>
+      <c r="A4" s="33" t="s">
+        <v>100</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="62" t="s">
-        <v>125</v>
+      <c r="D4" s="41" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
-        <v>120</v>
+      <c r="A5" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>124</v>
+      <c r="D5" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60" t="s">
-        <v>119</v>
+      <c r="D7" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="54" t="s">
-        <v>126</v>
-      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>119</v>
+      <c r="A9" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="65" t="s">
-        <v>128</v>
-      </c>
+      <c r="D9" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>121</v>
+      <c r="A10" s="34" t="s">
+        <v>104</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>94</v>
+      <c r="D10" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
-        <v>121</v>
+      <c r="A11" s="34" t="s">
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>94</v>
+      <c r="D11" s="5" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
-        <v>119</v>
+      <c r="A12" s="35" t="s">
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>94</v>
-      </c>
+      <c r="D12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="65"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="A13" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>72</v>
+      <c r="D13" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="53"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>57</v>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="D15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="53"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="D16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="53"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="D17" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="32"/>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="53"/>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="53"/>
-      <c r="C20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="53"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="52" t="s">
-        <v>48</v>
+      <c r="D21" s="16" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="53"/>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="52" t="s">
-        <v>48</v>
+      <c r="D22" s="16" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="53"/>
-      <c r="C23" s="64" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>69</v>
+      <c r="D23" s="40" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="15" t="s">
         <v>31</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="K34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="16" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="J36" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="K36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="J37" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7"/>
+      <c r="D37" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="J37" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
     </row>
     <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J38" s="9"/>
-      <c r="M38" s="32" t="s">
-        <v>61</v>
+      <c r="D38" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J38" s="8"/>
+      <c r="M38" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="N38" t="s">
-        <v>86</v>
-      </c>
-      <c r="P38" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="P38" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>85</v>
+      </c>
+      <c r="S38" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="Q38" t="s">
-        <v>86</v>
-      </c>
-      <c r="S38" s="32" t="s">
-        <v>64</v>
-      </c>
       <c r="T38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="G39" s="16"/>
-      <c r="I39" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J39" s="9"/>
-      <c r="M39" s="34" t="s">
-        <v>62</v>
+      <c r="D39" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" s="62" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="44"/>
+      <c r="I39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J39" s="8"/>
+      <c r="M39" s="26" t="s">
+        <v>61</v>
       </c>
       <c r="N39" t="s">
-        <v>86</v>
-      </c>
-      <c r="S39" s="33" t="s">
-        <v>65</v>
+        <v>85</v>
+      </c>
+      <c r="S39" s="25" t="s">
+        <v>64</v>
       </c>
       <c r="T39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="F40" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="J40" s="9"/>
+      <c r="D40" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F40" s="44"/>
+      <c r="I40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J40" s="8"/>
     </row>
     <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="F41" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41" s="9"/>
+      <c r="D41" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J41" s="8"/>
     </row>
     <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="49"/>
-      <c r="H42" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" s="15"/>
+      <c r="D42" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" s="45"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="J42" s="47"/>
       <c r="K42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>91</v>
-      </c>
-      <c r="F43" s="48"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="J43" s="15"/>
+      <c r="D43" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" s="43"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="J43" s="47"/>
       <c r="K43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F44" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="H44" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J44" s="15"/>
+      <c r="D44" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="H44" s="45"/>
+      <c r="I44" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="47"/>
       <c r="K44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="55" t="s">
-        <v>126</v>
+      <c r="D45" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="H45" s="45"/>
-      <c r="I45" s="18" t="s">
+      <c r="I45" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="J45" s="49"/>
+      <c r="K45" t="s">
         <v>85</v>
-      </c>
-      <c r="J45" s="19"/>
-      <c r="K45" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F46" s="56" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="I46" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="J46" s="23"/>
+      <c r="D46" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H46" s="44"/>
+      <c r="I46" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="J46" s="51"/>
       <c r="K46" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="57" t="s">
-        <v>117</v>
+      <c r="A47" s="33" t="s">
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E47" s="28" t="s">
+      <c r="D47" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="H47" s="43"/>
+      <c r="I47" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="I47" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="J47" s="23"/>
-    </row>
-    <row r="48" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J47" s="51"/>
+    </row>
+    <row r="48" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="I48" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="J48" s="23"/>
+      <c r="D48" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="H48" s="43"/>
+      <c r="I48" s="54" t="s">
+        <v>90</v>
+      </c>
+      <c r="J48" s="55"/>
     </row>
     <row r="49" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="F49" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="J49" s="25"/>
-    </row>
-    <row r="50" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="43"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="J49" s="57"/>
+    </row>
+    <row r="50" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="F50" s="58" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I56" s="8" t="s">
+      <c r="D50" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" s="53"/>
+    </row>
+    <row r="51" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J51" s="18"/>
+    </row>
+    <row r="52" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
+      <c r="I52" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J52" s="18"/>
+    </row>
+    <row r="53" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="J53" s="20"/>
+    </row>
+    <row r="66" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I67" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="9"/>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I57" s="10" t="s">
+      <c r="J67" s="8"/>
+    </row>
+    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I68" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J57" s="11"/>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I58" s="10" t="s">
+      <c r="J68" s="10"/>
+    </row>
+    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I69" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J58" s="11"/>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I59" s="10" t="s">
+      <c r="J69" s="10"/>
+    </row>
+    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I70" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J59" s="11"/>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I60" s="10" t="s">
+      <c r="J70" s="10"/>
+    </row>
+    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I71" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J60" s="11"/>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I61" s="10" t="s">
+      <c r="J71" s="10"/>
+    </row>
+    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I72" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J61" s="11"/>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I62" s="10" t="s">
+      <c r="J72" s="10"/>
+    </row>
+    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I73" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J62" s="11"/>
-    </row>
-    <row r="63" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I63" s="12" t="s">
+      <c r="J73" s="10"/>
+    </row>
+    <row r="74" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I74" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J63" s="13"/>
+      <c r="J74" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
feat: version alpha 0.1 complete -complete core components overhaul -telemetry endpoint with buffer waiting for server integration -complete hmi menu in testing phase -create multiple helper libraries
</commit_message>
<xml_diff>
--- a/PINOUT.xlsx
+++ b/PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Projects\WS_Solarium_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F90898-5DCC-4121-849E-EB7B869A25EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AAC869-E184-4D95-8E5F-78F4C2359E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25920" yWindow="3405" windowWidth="12480" windowHeight="15345" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
+    <workbookView xWindow="27495" yWindow="5580" windowWidth="12480" windowHeight="15345" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="131">
   <si>
     <t>GPIO1</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>PWM - SERVO - YAW CTRL</t>
+  </si>
+  <si>
+    <t>next to GPIO45</t>
+  </si>
+  <si>
+    <t>3V3_HALL_ARRAY_TOGGLE</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,12 +636,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFDFBD3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF3F0F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -864,7 +864,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -929,7 +929,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1262,7 +1261,7 @@
   <dimension ref="A1:T74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,6 +1303,9 @@
       <c r="E2" s="59" t="s">
         <v>86</v>
       </c>
+      <c r="F2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
@@ -1381,8 +1383,8 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="64" t="s">
-        <v>48</v>
+      <c r="D9" s="39" t="s">
+        <v>130</v>
       </c>
       <c r="E9" s="13"/>
     </row>
@@ -1421,7 +1423,7 @@
       <c r="D12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="65"/>
+      <c r="E12" s="64"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">

</xml_diff>

<commit_message>
refactor: modularize components, fix bugs, simplify architecture
</commit_message>
<xml_diff>
--- a/PINOUT.xlsx
+++ b/PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Projects\WS_Solarium_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AAC869-E184-4D95-8E5F-78F4C2359E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D75AF85-A073-4982-91F9-70128DE35427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27495" yWindow="5580" windowWidth="12480" windowHeight="15345" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>GPIO1</t>
   </si>
@@ -183,9 +183,6 @@
     <t>GPIO48</t>
   </si>
   <si>
-    <t>FREE</t>
-  </si>
-  <si>
     <t>MCP3208 ADC CH. 1</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>PWM - CC LED driver</t>
   </si>
   <si>
-    <t>PWM - case cooling fan</t>
-  </si>
-  <si>
     <t>ADS1115 ADC 3 CH. 1 - MT</t>
   </si>
   <si>
@@ -354,18 +348,6 @@
     <t>BOTH Boot/Flash</t>
   </si>
   <si>
-    <t>SN74AHCT125's OE #1</t>
-  </si>
-  <si>
-    <t>SN74AHCT125's OE #2</t>
-  </si>
-  <si>
-    <t>HALL DI - Rainfall Water input</t>
-  </si>
-  <si>
-    <t>HALL DI - Rain Tipbucket</t>
-  </si>
-  <si>
     <t>ADS1115 ADC 4 CH. 1 - HALL</t>
   </si>
   <si>
@@ -381,62 +363,100 @@
     <t>SPI DC - OLED</t>
   </si>
   <si>
-    <t>?</t>
+    <t>3V3_SENSOR_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 5</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 4</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 3</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 2</t>
+  </si>
+  <si>
+    <t>MOSFET - TOGGLE Valve 1</t>
+  </si>
+  <si>
+    <t>MOSFET - PWM PUMP</t>
+  </si>
+  <si>
+    <t>UART TX - PMS5003</t>
+  </si>
+  <si>
+    <t>UART RX - PMS5003</t>
+  </si>
+  <si>
+    <t>PWM - SERVO - PITCH CTRL</t>
+  </si>
+  <si>
+    <t>PWM - SERVO - YAW CTRL</t>
+  </si>
+  <si>
+    <t>next to GPIO45</t>
+  </si>
+  <si>
+    <t>3V3_HALL_ARRAY_TOGGLE</t>
+  </si>
+  <si>
+    <t>PWM - 12V cooling fan</t>
+  </si>
+  <si>
+    <t>12V_FAN_TOGGLE</t>
+  </si>
+  <si>
+    <r>
+      <t>5V_BUS_TOGGLE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - OD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6V6_BUS_TOGGLE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - OD</t>
+    </r>
+  </si>
+  <si>
+    <t>HALL DI - Rainfall Tipbucket</t>
+  </si>
+  <si>
+    <t>HALL DI - Tank water intake</t>
+  </si>
+  <si>
+    <t>Octal SPI PSRAM</t>
   </si>
   <si>
     <t>12V_BUS_TOGGLE</t>
-  </si>
-  <si>
-    <t>6V6_BUS_TOGGLE</t>
-  </si>
-  <si>
-    <t>5V_BUS_TOGGLE</t>
-  </si>
-  <si>
-    <t>3V3_SENSOR_BUS_TOGGLE</t>
-  </si>
-  <si>
-    <t>MOSFET - TOGGLE Valve 5</t>
-  </si>
-  <si>
-    <t>MOSFET - TOGGLE Valve 4</t>
-  </si>
-  <si>
-    <t>MOSFET - TOGGLE Valve 3</t>
-  </si>
-  <si>
-    <t>MOSFET - TOGGLE Valve 2</t>
-  </si>
-  <si>
-    <t>MOSFET - TOGGLE Valve 1</t>
-  </si>
-  <si>
-    <t>MOSFET - PWM PUMP</t>
-  </si>
-  <si>
-    <t>UART TX - PMS5003</t>
-  </si>
-  <si>
-    <t>UART RX - PMS5003</t>
-  </si>
-  <si>
-    <t>PWM - SERVO - PITCH CTRL</t>
-  </si>
-  <si>
-    <t>PWM - SERVO - YAW CTRL</t>
-  </si>
-  <si>
-    <t>next to GPIO45</t>
-  </si>
-  <si>
-    <t>3V3_HALL_ARRAY_TOGGLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,8 +507,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF6B3109"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,12 +671,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA66BD3"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -635,12 +689,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDFBD3"/>
+        <fgColor rgb="FFFF8585"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -860,11 +914,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF7030A0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF7030A0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF7030A0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF7030A0"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -892,44 +1007,49 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,16 +1058,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF8585"/>
+      <color rgb="FFA66BD3"/>
+      <color rgb="FF6B3109"/>
       <color rgb="FFF3F0F4"/>
       <color rgb="FFFDFBD3"/>
       <color rgb="FFD5B6EC"/>
       <color rgb="FFBF94E0"/>
       <color rgb="FFDAC0EE"/>
-      <color rgb="FFA66BD3"/>
       <color rgb="FF85FFBC"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FF7CB854"/>
-      <color rgb="FF3B9B40"/>
     </mruColors>
   </colors>
   <extLst>
@@ -959,6 +1079,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>341629</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>649694</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3FCFB49-AE79-4C91-9996-51C25696EEDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8980804" y="95467"/>
+          <a:ext cx="10528390" cy="7181633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986543E9-FEEA-4416-9297-1960C94E5E52}">
-  <dimension ref="A1:T74"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,705 +1465,663 @@
     <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="B3" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>100</v>
-      </c>
+      <c r="D3" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
-        <v>103</v>
-      </c>
+      <c r="D4" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="66"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="33"/>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="39" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>102</v>
-      </c>
+      <c r="D7" s="63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="32"/>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="39" t="s">
-        <v>115</v>
+      <c r="D8" s="63" t="s">
+        <v>128</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>102</v>
-      </c>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="32"/>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="39" t="s">
-        <v>130</v>
+      <c r="D9" s="54" t="s">
+        <v>120</v>
       </c>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>104</v>
-      </c>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="31"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>104</v>
-      </c>
+      <c r="D10" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="31"/>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
-        <v>102</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="32"/>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="64"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>102</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E12" s="53"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="32"/>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="29"/>
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="29"/>
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
       <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="29"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
       <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="29"/>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
+      <c r="H18" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="29"/>
       <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
+        <v>64</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
+        <v>66</v>
+      </c>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="H20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="29"/>
       <c r="C21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32"/>
+      <c r="D21" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="K21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="O21" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q21" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
       <c r="C22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="38" t="s">
+      <c r="D22" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="K22" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q22" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="29"/>
+      <c r="C23" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D23" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F24" s="36"/>
+      <c r="G24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F25" s="37"/>
+      <c r="G25" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F26" s="37"/>
+      <c r="G26" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="40"/>
+      <c r="I26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F27" s="38"/>
+      <c r="G27" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F28" s="38"/>
+      <c r="G28" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="42"/>
+      <c r="I28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F29" s="37"/>
+      <c r="G29" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="44"/>
+      <c r="I29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F30" s="36"/>
+      <c r="G30" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="44"/>
+    </row>
+    <row r="31" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F31" s="36"/>
+      <c r="G31" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" s="48"/>
+    </row>
+    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F32" s="36"/>
+      <c r="G32" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" s="50"/>
+    </row>
+    <row r="33" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F33" s="36"/>
+      <c r="G33" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="H33" s="46"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F34" s="36"/>
+      <c r="G34" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J35" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="36"/>
+      <c r="G35" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="J36" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="K36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="36"/>
+      <c r="G36" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="J37" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-    </row>
-    <row r="38" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="58" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="8"/>
-      <c r="M38" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="N38" t="s">
-        <v>85</v>
-      </c>
-      <c r="P38" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>85</v>
-      </c>
-      <c r="S38" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="T38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="R38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="44"/>
-      <c r="I39" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="J39" s="8"/>
-      <c r="M39" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="N39" t="s">
-        <v>85</v>
-      </c>
-      <c r="S39" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="T39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="R39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="44"/>
-      <c r="I40" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="J42" s="47"/>
-      <c r="K42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="G43" s="43"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" s="47"/>
-      <c r="K43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="H44" s="45"/>
-      <c r="I44" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="J44" s="47"/>
-      <c r="K44" t="s">
+      <c r="D44" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="61" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="45"/>
-      <c r="I45" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="J45" s="49"/>
-      <c r="K45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H46" s="44"/>
-      <c r="I46" s="50" t="s">
-        <v>89</v>
-      </c>
-      <c r="J46" s="51"/>
-      <c r="K46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="33" t="s">
-        <v>100</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="30"/>
       <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="59" t="s">
+      <c r="D47" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="H47" s="43"/>
-      <c r="I47" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="J47" s="51"/>
-    </row>
-    <row r="48" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="36"/>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="H48" s="43"/>
-      <c r="I48" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="J48" s="55"/>
-    </row>
-    <row r="49" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="E48" s="61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="E49" s="43"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="J49" s="57"/>
-    </row>
-    <row r="50" spans="3:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="36"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="J50" s="53"/>
-    </row>
-    <row r="51" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J51" s="18"/>
-    </row>
-    <row r="52" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="J52" s="18"/>
-    </row>
-    <row r="53" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="43"/>
-      <c r="I53" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="J53" s="20"/>
+      <c r="D50" s="55" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="66" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I66" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I67" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J67" s="8"/>
     </row>
     <row r="68" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I68" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J68" s="10"/>
     </row>
     <row r="69" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I69" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J69" s="10"/>
     </row>
     <row r="70" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I70" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J70" s="10"/>
     </row>
     <row r="71" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I71" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J71" s="10"/>
     </row>
     <row r="72" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I72" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J72" s="10"/>
     </row>
     <row r="73" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I73" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J73" s="10"/>
     </row>
     <row r="74" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I74" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J74" s="12"/>
     </row>
@@ -1985,5 +2129,6 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: minor bug fixes and optimizations throughout
</commit_message>
<xml_diff>
--- a/PINOUT.xlsx
+++ b/PINOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Projects\WS_Solarium_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D75AF85-A073-4982-91F9-70128DE35427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637A635-A44F-4F4C-81D1-791595D98695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="135">
   <si>
     <t>GPIO1</t>
   </si>
@@ -216,21 +216,6 @@
     <t>ADC2</t>
   </si>
   <si>
-    <t>BME280</t>
-  </si>
-  <si>
-    <t>SHT40</t>
-  </si>
-  <si>
-    <t>AS5600</t>
-  </si>
-  <si>
-    <t>INA219</t>
-  </si>
-  <si>
-    <t>SEN291</t>
-  </si>
-  <si>
     <t>ENCODER CLK</t>
   </si>
   <si>
@@ -252,12 +237,6 @@
     <t>SPID MOSI</t>
   </si>
   <si>
-    <t>I2C SDA</t>
-  </si>
-  <si>
-    <t>I2C SCL</t>
-  </si>
-  <si>
     <t>alternative</t>
   </si>
   <si>
@@ -279,9 +258,6 @@
     <t>ADS1115 ADC 3 CH. 4 - FREE</t>
   </si>
   <si>
-    <t>ADS1115 ADC 2 CH. 1 - MT</t>
-  </si>
-  <si>
     <t>ADS1115 ADC 2 CH. 2 - MT</t>
   </si>
   <si>
@@ -300,12 +276,6 @@
     <t>PWM - CC LED driver</t>
   </si>
   <si>
-    <t>ADS1115 ADC 3 CH. 1 - MT</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 3 - FREE</t>
-  </si>
-  <si>
     <t>ADS1115 ADC 3 CH. 2 - PT - pump</t>
   </si>
   <si>
@@ -318,12 +288,6 @@
     <t>ADS1115 ADC 1 CH. 2 - PR</t>
   </si>
   <si>
-    <t>ADS1115 ADC 1 CH. 1 - PR</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pin </t>
   </si>
   <si>
@@ -337,18 +301,6 @@
   </si>
   <si>
     <t>Warnings:</t>
-  </si>
-  <si>
-    <t>Flash-Connected Pin</t>
-  </si>
-  <si>
-    <t>UART0 Pin</t>
-  </si>
-  <si>
-    <t>BOTH Boot/Flash</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 4 CH. 1 - HALL</t>
   </si>
   <si>
     <t>ADS1115 ADC 4 CH. 2 - HALL</t>
@@ -451,12 +403,78 @@
   <si>
     <t>12V_BUS_TOGGLE</t>
   </si>
+  <si>
+    <t>USB_D-</t>
+  </si>
+  <si>
+    <t>UART0</t>
+  </si>
+  <si>
+    <t>ADS1115 ADCs:</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 3 CH. 3 - 3V3 BUS</t>
+  </si>
+  <si>
+    <t>I2C SCL (temporary)</t>
+  </si>
+  <si>
+    <t>I2C SDA (temporary)</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 1 CH. 1 - PR 0x48</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 2 CH. 1 - MT 0x49</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 3 CH. 1 - MT 0x4A</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 4 CH. 1 - HALL 0x4B</t>
+  </si>
+  <si>
+    <t>BME280 0x76</t>
+  </si>
+  <si>
+    <t>AS5600 0x36</t>
+  </si>
+  <si>
+    <t>INA219 0x40</t>
+  </si>
+  <si>
+    <t>SEN291 0x41</t>
+  </si>
+  <si>
+    <t>SHT40     0x44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP23008 0x20 </t>
+  </si>
+  <si>
+    <t>Future plan!</t>
+  </si>
+  <si>
+    <t>Chip boot mode</t>
+  </si>
+  <si>
+    <t>JTAG signal source</t>
+  </si>
+  <si>
+    <t>ROM message print</t>
+  </si>
+  <si>
+    <t>VDD_SPI voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Chip boot mode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +565,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -605,12 +639,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEADBF5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -659,31 +687,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA66BD3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBF94E0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD5B6EC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,8 +697,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7A2B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3A36D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7C5A3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -813,19 +847,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -849,54 +870,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFFF0000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -975,11 +948,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -997,59 +1101,81 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,16 +1184,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFED7A2B"/>
+      <color rgb="FFF3A36D"/>
+      <color rgb="FFF7C5A3"/>
+      <color rgb="FFC65911"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFFF8585"/>
       <color rgb="FFA66BD3"/>
       <color rgb="FF6B3109"/>
       <color rgb="FFF3F0F4"/>
       <color rgb="FFFDFBD3"/>
-      <color rgb="FFD5B6EC"/>
-      <color rgb="FFBF94E0"/>
-      <color rgb="FFDAC0EE"/>
-      <color rgb="FF85FFBC"/>
-      <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1086,15 +1212,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>341629</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95467</xdr:rowOff>
+      <xdr:colOff>855979</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>649694</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>402044</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1124,7 +1250,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8980804" y="95467"/>
+          <a:off x="9495154" y="743167"/>
           <a:ext cx="10528390" cy="7181633"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1447,634 +1573,733 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>96</v>
+        <v>84</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>121</v>
+      <c r="A2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>103</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
-        <v>101</v>
-      </c>
+      <c r="A3" s="22"/>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" s="65" t="s">
-        <v>85</v>
+      <c r="D3" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="30"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="66"/>
+      <c r="D4" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="43"/>
+      <c r="H4" s="16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="33"/>
+      <c r="A5" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="85" t="s">
+        <v>131</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>125</v>
-      </c>
+      <c r="D5" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="84"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="64" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="65"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="63" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" s="32"/>
+      <c r="D7" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="64" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="65"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="32"/>
+      <c r="D8" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="67"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="61" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="31"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>126</v>
-      </c>
+      <c r="E10" s="84"/>
+      <c r="G10" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="31"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="32"/>
+      <c r="E11" s="22"/>
+      <c r="G11" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="53"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="32"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" s="59"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="60"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="60"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="68"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="H17" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F17" s="13"/>
+      <c r="G17" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" s="70"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="21" t="s">
-        <v>65</v>
-      </c>
+      <c r="D18" s="17"/>
       <c r="E18" s="13"/>
-      <c r="H18" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="71"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
       <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
+      <c r="D19" s="17"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="71"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="H20" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="29"/>
-      <c r="C21" s="4" t="s">
+      <c r="D20" s="17"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="73"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49"/>
+      <c r="B21" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="K21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="L21" t="s">
-        <v>84</v>
-      </c>
-      <c r="N21" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="O21" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q21" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="29"/>
-      <c r="C22" s="4" t="s">
+      <c r="D21" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="74"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="K22" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="L22" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29"/>
-      <c r="C23" s="34" t="s">
+      <c r="D22" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="75"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="22"/>
+      <c r="C23" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="26"/>
+      <c r="G24" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="37"/>
-      <c r="G25" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="40"/>
-      <c r="I25" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="77"/>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="37"/>
-      <c r="G26" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="H26" s="40"/>
-      <c r="I26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="77"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="40"/>
-      <c r="I27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="27"/>
+      <c r="G27" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" s="42"/>
-      <c r="I28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="27"/>
+      <c r="G28" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="37"/>
-      <c r="G29" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="H29" s="44"/>
-      <c r="I29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="77"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="44"/>
-    </row>
-    <row r="31" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="76"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="36"/>
-      <c r="G31" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="H31" s="48"/>
-    </row>
-    <row r="32" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F31" s="26"/>
+      <c r="G31" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" s="50"/>
-    </row>
-    <row r="33" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="76"/>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="H33" s="46"/>
+      <c r="F33" s="76"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H34" s="18"/>
-    </row>
-    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="26"/>
+      <c r="G34" s="82" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C35" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="H35" s="18"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="80"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="36"/>
-      <c r="G36" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36" s="20"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="75"/>
+      <c r="H36" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="37" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="35"/>
       <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="58" t="s">
-        <v>127</v>
+      <c r="D37" s="35" t="s">
+        <v>111</v>
       </c>
       <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="75"/>
+      <c r="H37" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="45"/>
       <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="68" t="s">
-        <v>127</v>
+      <c r="D38" s="45" t="s">
+        <v>111</v>
       </c>
       <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="75"/>
+      <c r="H38" t="s">
+        <v>129</v>
+      </c>
       <c r="R38" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="36"/>
       <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="59" t="s">
-        <v>127</v>
+      <c r="D39" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="75"/>
+      <c r="H39" t="s">
+        <v>129</v>
       </c>
       <c r="R39" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="51" t="s">
-        <v>113</v>
-      </c>
-      <c r="E40" s="52" t="s">
-        <v>85</v>
+      <c r="D40" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="75"/>
+      <c r="H40" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="27" t="s">
-        <v>112</v>
+      <c r="D41" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="75"/>
+      <c r="H41" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="27" t="s">
-        <v>111</v>
+      <c r="D42" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="75"/>
+      <c r="H42" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="27" t="s">
-        <v>110</v>
+      <c r="D43" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="75"/>
+      <c r="H43" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" s="61" t="s">
-        <v>85</v>
+      <c r="D44" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="75"/>
+      <c r="H44" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C45" s="2" t="s">
+      <c r="A45" s="50"/>
+      <c r="B45" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="47" t="s">
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G45" s="75"/>
+      <c r="H45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="50"/>
+      <c r="B46" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="48" t="s">
         <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>116</v>
+        <v>100</v>
+      </c>
+      <c r="G46" s="75"/>
+      <c r="H46" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="26"/>
+      <c r="G47" s="75"/>
+      <c r="H47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="91" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="36"/>
-    </row>
-    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="E48" s="61" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="75"/>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="89"/>
+      <c r="B49" s="90" t="s">
+        <v>134</v>
+      </c>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" s="36"/>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="26"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="55" t="s">
-        <v>117</v>
-      </c>
+      <c r="D50" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J50" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="L50" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H51" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H52" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J56" s="13"/>
     </row>
     <row r="66" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I66" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="9:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactor: major overhaul and bug fixes
</commit_message>
<xml_diff>
--- a/PINOUT.xlsx
+++ b/PINOUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\Projects\WS_Solarium_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6637A635-A44F-4F4C-81D1-791595D98695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD41E1C-CC70-4A13-8374-C248533BFD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9FCD7DAD-4811-4693-9C9B-A0B0FCD3B9C5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="140">
   <si>
     <t>GPIO1</t>
   </si>
@@ -216,15 +216,6 @@
     <t>ADC2</t>
   </si>
   <si>
-    <t>ENCODER CLK</t>
-  </si>
-  <si>
-    <t>ENCODER DAT</t>
-  </si>
-  <si>
-    <t>ENCODER SW</t>
-  </si>
-  <si>
     <t>1 WIRE - DS18B20</t>
   </si>
   <si>
@@ -246,15 +237,6 @@
     <t>SPI CS1 - OLED</t>
   </si>
   <si>
-    <t>Pressure pump</t>
-  </si>
-  <si>
-    <t>4x Photoresistor</t>
-  </si>
-  <si>
-    <t>5x Moisture sensor</t>
-  </si>
-  <si>
     <t>ADS1115 ADC 3 CH. 4 - FREE</t>
   </si>
   <si>
@@ -270,9 +252,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>SN74AHCT125</t>
-  </si>
-  <si>
     <t>PWM - CC LED driver</t>
   </si>
   <si>
@@ -315,9 +294,6 @@
     <t>SPI DC - OLED</t>
   </si>
   <si>
-    <t>3V3_SENSOR_BUS_TOGGLE</t>
-  </si>
-  <si>
     <t>MOSFET - TOGGLE Valve 5</t>
   </si>
   <si>
@@ -348,12 +324,6 @@
     <t>PWM - SERVO - YAW CTRL</t>
   </si>
   <si>
-    <t>next to GPIO45</t>
-  </si>
-  <si>
-    <t>3V3_HALL_ARRAY_TOGGLE</t>
-  </si>
-  <si>
     <t>PWM - 12V cooling fan</t>
   </si>
   <si>
@@ -361,7 +331,7 @@
   </si>
   <si>
     <r>
-      <t>5V_BUS_TOGGLE</t>
+      <t>6V6_BUS_TOGGLE</t>
     </r>
     <r>
       <rPr>
@@ -376,14 +346,86 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>6V6_BUS_TOGGLE</t>
+    <t>Octal SPI PSRAM</t>
+  </si>
+  <si>
+    <t>12V_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <t>USB_D-</t>
+  </si>
+  <si>
+    <t>UART0</t>
+  </si>
+  <si>
+    <t>ADS1115 ADC 3 CH. 3 - 3V3 BUS</t>
+  </si>
+  <si>
+    <t>INA219 0x40</t>
+  </si>
+  <si>
+    <t>SEN291 0x41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP23008 0x20 </t>
+  </si>
+  <si>
+    <t>Chip boot mode</t>
+  </si>
+  <si>
+    <t>JTAG signal source</t>
+  </si>
+  <si>
+    <t>ROM message print</t>
+  </si>
+  <si>
+    <t>VDD_SPI voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Chip boot mode</t>
+  </si>
+  <si>
+    <t>MCP23008 INTR</t>
+  </si>
+  <si>
+    <t>(next to GPIO45)</t>
+  </si>
+  <si>
+    <t>I2C_NUM_0 SDA</t>
+  </si>
+  <si>
+    <t>I2C_NUM_0 SCL</t>
+  </si>
+  <si>
+    <t>I2C_NUM_1 SDA</t>
+  </si>
+  <si>
+    <t>I2C_NUM_1 SCL</t>
+  </si>
+  <si>
+    <t>I2C_NUM0</t>
+  </si>
+  <si>
+    <t>I2C_NUM1</t>
+  </si>
+  <si>
+    <t>SN74AHCT125#0</t>
+  </si>
+  <si>
+    <t>SN74AHCT125#1</t>
+  </si>
+  <si>
+    <t>5V_BUS_TOGGLE</t>
+  </si>
+  <si>
+    <r>
+      <t>3V3_SENSOR_BUS_TOGGLE</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="4" tint="-0.499984740745262"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -392,89 +434,264 @@
     </r>
   </si>
   <si>
-    <t>HALL DI - Rainfall Tipbucket</t>
-  </si>
-  <si>
-    <t>HALL DI - Tank water intake</t>
-  </si>
-  <si>
-    <t>Octal SPI PSRAM</t>
-  </si>
-  <si>
-    <t>12V_BUS_TOGGLE</t>
-  </si>
-  <si>
-    <t>USB_D-</t>
-  </si>
-  <si>
-    <t>UART0</t>
-  </si>
-  <si>
-    <t>ADS1115 ADCs:</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 3 - 3V3 BUS</t>
-  </si>
-  <si>
-    <t>I2C SCL (temporary)</t>
-  </si>
-  <si>
-    <t>I2C SDA (temporary)</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 1 CH. 1 - PR 0x48</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 2 CH. 1 - MT 0x49</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 3 CH. 1 - MT 0x4A</t>
-  </si>
-  <si>
-    <t>ADS1115 ADC 4 CH. 1 - HALL 0x4B</t>
-  </si>
-  <si>
-    <t>BME280 0x76</t>
-  </si>
-  <si>
-    <t>AS5600 0x36</t>
-  </si>
-  <si>
-    <t>INA219 0x40</t>
-  </si>
-  <si>
-    <t>SEN291 0x41</t>
-  </si>
-  <si>
-    <t>SHT40     0x44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP23008 0x20 </t>
-  </si>
-  <si>
-    <t>Future plan!</t>
-  </si>
-  <si>
-    <t>Chip boot mode</t>
-  </si>
-  <si>
-    <t>JTAG signal source</t>
-  </si>
-  <si>
-    <t>ROM message print</t>
-  </si>
-  <si>
-    <t>VDD_SPI voltage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +Chip boot mode</t>
+    <t>SN74AHCT125N Output EN - OD</t>
+  </si>
+  <si>
+    <t>9 act 26 sens 7 helping devs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BME280 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x76</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SHT40     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x44</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AS5600 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x36</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADS1115 ADC 4 CH. 1 - HALL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x4B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADS1115 ADC 2 CH. 1 - MT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x48 -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> DEV#0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADS1115 ADC 3 CH. 1 - MT </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x49 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- DEV#1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ADS1115 ADC 1 CH. 1 - PR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x4A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HALL DI - Rainfall Tipbucket</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - GP3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>HALL DI - Tank water intake</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - GP4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ENCODER CLK</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - GP1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ENCODER DAT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - GP0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ENCODER SW</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -  GP2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3V3_HALL_ARRAY_TOGGLE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - GP5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SPI OLED RESET - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GP6</t>
+    </r>
+  </si>
+  <si>
+    <t>WS2812 LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,8 +798,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFBF5311"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,8 +983,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3E6CC0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAABFE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9A4E4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -995,7 +1275,55 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -1007,6 +1335,17 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
@@ -1017,65 +1356,105 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color theme="9"/>
+      </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="mediumDashed">
+        <color theme="9"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color theme="9"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color theme="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1083,13 +1462,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1098,84 +1475,110 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1184,16 +1587,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC9A4E4"/>
+      <color rgb="FFBF5311"/>
+      <color rgb="FFED7A33"/>
+      <color rgb="FFAABFE4"/>
+      <color rgb="FF3E6CC0"/>
+      <color rgb="FFEC7524"/>
+      <color rgb="FFEF863F"/>
       <color rgb="FFED7A2B"/>
       <color rgb="FFF3A36D"/>
       <color rgb="FFF7C5A3"/>
-      <color rgb="FFC65911"/>
-      <color rgb="FF00FFFF"/>
-      <color rgb="FFFF8585"/>
-      <color rgb="FFA66BD3"/>
-      <color rgb="FF6B3109"/>
-      <color rgb="FFF3F0F4"/>
-      <color rgb="FFFDFBD3"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1212,15 +1615,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>855979</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>152617</xdr:rowOff>
+      <xdr:colOff>417829</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114517</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>402044</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>583019</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1250,7 +1653,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9495154" y="743167"/>
+          <a:off x="11228704" y="2133817"/>
           <a:ext cx="10528390" cy="7181633"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1573,782 +1976,769 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>108</v>
+        <v>80</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="D3" s="63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="53"/>
+      <c r="F3" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="78"/>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="43"/>
-      <c r="H4" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="85" t="s">
-        <v>131</v>
+      <c r="D4" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="42"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="77" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="H5" s="63"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="39"/>
+      <c r="G5" s="65" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="65"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="95" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="98"/>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="H7" s="65"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="D7" s="96" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="67"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="D8" s="96" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="100"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="104" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" s="62"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="D9" s="97" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="101"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="112" t="s">
+        <v>137</v>
+      </c>
+      <c r="J9" s="113" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="G10" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="62"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="D10" s="94" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="111" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="G11" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="62"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="109" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="61" t="s">
+      <c r="E12" s="20"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="H15" s="82"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="H16" s="82"/>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="72"/>
+      <c r="F17" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="82"/>
+    </row>
+    <row r="18" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="92" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="81"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="14"/>
+      <c r="C20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="91" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="H20" s="36"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="37"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="Q21" s="11"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="34"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="14"/>
+      <c r="C23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="107" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="34"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="103" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="34"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="H26" s="32"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="62"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="59"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-      <c r="C14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="60"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="57" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" s="60"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22"/>
-      <c r="C16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="H17" s="70"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="58" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" s="71"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" s="71"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22"/>
-      <c r="C20" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" s="73"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="74"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="Q21" s="13"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="49"/>
-      <c r="B22" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="75"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22"/>
-      <c r="C23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="77"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="77"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="27"/>
-      <c r="G27" s="18" t="s">
+      <c r="H27" s="33"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="33"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="41"/>
+      <c r="G29" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" s="38"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" s="40"/>
+      <c r="G30" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="H30" s="62"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="H31" s="60"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="40"/>
+      <c r="G32" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" s="60"/>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="40"/>
+      <c r="G33" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="61"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="40"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="39"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="39"/>
+      <c r="G36" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="27"/>
-      <c r="G28" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="77"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="76"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="76"/>
-    </row>
-    <row r="33" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F33" s="76"/>
-    </row>
-    <row r="34" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="82" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C35" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="80"/>
-    </row>
-    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="75"/>
-      <c r="H36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35"/>
+    <row r="37" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
       <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="75"/>
-      <c r="H37" t="s">
-        <v>129</v>
+      <c r="D37" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="76" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="45"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="75"/>
-      <c r="H38" t="s">
-        <v>129</v>
-      </c>
+      <c r="D38" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="39"/>
       <c r="R38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="36"/>
+      <c r="B39" s="22"/>
       <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="75"/>
-      <c r="H39" t="s">
-        <v>129</v>
-      </c>
+      <c r="D39" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="39"/>
+      <c r="G39" s="72"/>
       <c r="R39" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="75"/>
-      <c r="H40" t="s">
-        <v>129</v>
-      </c>
+      <c r="D40" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="39"/>
+      <c r="G40" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="75"/>
-      <c r="H41" t="s">
-        <v>129</v>
-      </c>
+      <c r="D41" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="75"/>
-      <c r="H42" t="s">
-        <v>129</v>
-      </c>
+      <c r="D42" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="75"/>
-      <c r="H43" t="s">
-        <v>129</v>
-      </c>
+      <c r="D43" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
     </row>
     <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="75"/>
-      <c r="H44" t="s">
-        <v>129</v>
-      </c>
+      <c r="D44" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="17"/>
+      <c r="K44" s="11"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="47" t="s">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G45" s="75"/>
-      <c r="H45" t="s">
-        <v>129</v>
-      </c>
+      <c r="D45" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="17"/>
     </row>
     <row r="46" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
-      <c r="B46" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="48" t="s">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G46" s="75"/>
-      <c r="H46" t="s">
-        <v>129</v>
-      </c>
+      <c r="D46" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="17"/>
     </row>
     <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="86" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="86" t="s">
-        <v>133</v>
-      </c>
-      <c r="C47" s="87" t="s">
+      <c r="A47" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D47" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="E47" s="26"/>
-      <c r="G47" s="75"/>
-      <c r="H47" t="s">
-        <v>129</v>
-      </c>
+      <c r="D47" s="89" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="17"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="17"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="88" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="91" t="s">
+      <c r="A48" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="G48" s="75"/>
-    </row>
-    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="89"/>
-      <c r="B49" s="90" t="s">
-        <v>134</v>
+      <c r="D48" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" s="42"/>
+      <c r="G48" s="17"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="48"/>
+      <c r="B49" s="49" t="s">
+        <v>110</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="E49" s="26"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="81"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="2" t="s">
+      <c r="D49" s="84" t="s">
+        <v>94</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="105" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J50" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="L50" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H51" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="L51" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H52" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J56" s="13"/>
+      <c r="D50" s="90" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="11"/>
     </row>
     <row r="66" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I67" s="7" t="s">
+      <c r="I67" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J67" s="8"/>
+      <c r="J67" s="6"/>
     </row>
     <row r="68" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I68" s="9" t="s">
+      <c r="I68" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J68" s="10"/>
+      <c r="J68" s="8"/>
     </row>
     <row r="69" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I69" s="9" t="s">
+      <c r="I69" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J69" s="10"/>
+      <c r="J69" s="8"/>
     </row>
     <row r="70" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I70" s="9" t="s">
+      <c r="I70" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J70" s="10"/>
+      <c r="J70" s="8"/>
     </row>
     <row r="71" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I71" s="9" t="s">
+      <c r="I71" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="J71" s="10"/>
+      <c r="J71" s="8"/>
     </row>
     <row r="72" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I72" s="9" t="s">
+      <c r="I72" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J72" s="10"/>
+      <c r="J72" s="8"/>
     </row>
     <row r="73" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I73" s="9" t="s">
+      <c r="I73" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J73" s="10"/>
+      <c r="J73" s="8"/>
     </row>
     <row r="74" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I74" s="11" t="s">
+      <c r="I74" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J74" s="12"/>
+      <c r="J74" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>